<commit_message>
Assignment 4 parallel sort
</commit_message>
<xml_diff>
--- a/Asgn_Parallel_Sort.xlsx
+++ b/Asgn_Parallel_Sort.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MSIS\2_Spring22\Info_6205_Algo\Assignments\Assignment4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MSIS\2_Spring22\Info_6205_Algo\Assignments\Assignment3\Assignment3_Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DE4D59-1D86-4EB5-9FDA-C9B8403A6750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE810109-1DF8-4A23-8E53-585A4CF88B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D2C3BF45-F247-4C5A-9DD1-349AC937C189}"/>
   </bookViews>
@@ -6532,7 +6532,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>